<commit_message>
added journal and author information
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kribin/Documents/Analytics/R/Disturbance Cues/Familiarity &amp; Kinship Donors/Dryad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF70D5AD-8D0A-204A-81D3-79CB61BC0749}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C895FC-95D8-564C-80A9-19046111C0AC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{3642892E-B6F8-6747-AAEE-FD57B64FD60E}"/>
+    <workbookView xWindow="400" yWindow="900" windowWidth="27640" windowHeight="16540" activeTab="1" xr2:uid="{3642892E-B6F8-6747-AAEE-FD57B64FD60E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="26">
   <si>
     <t>trial</t>
   </si>
@@ -106,12 +107,38 @@
   <si>
     <t>prop</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Forget the audience: Tadpoles release similar disturbance cues regardless of kinship or familiarity. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Behavioral Ecology and Sociobiology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. Kevin R. Bairos‑Novak*, Adam L. Crane, Gabrielle H. Achtymichuk, Jonathan Hsin, Ita A. E. Rivera-Hernández, Olena M. Simko, Theresa E. Wrynn, Douglas P. Chivers, &amp; Maud C. O. Ferrari.
+*Corresponding author affiliation: Department of Biology, University of Saskatchewan, Saskatoon, SK, Canada; Marine Biology and Aquaculture &amp; ARC Centre of Excellence for Coral Reef Studies, James Cook University, James Cook University, QLD 4811, Australia
+Corresponding author email: kevin.bairosnovak@my.jcu.edu.au</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,6 +153,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -215,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -243,6 +289,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE7D5FD-6C47-AD47-ABAD-599B61F5503C}">
   <dimension ref="A1:I380"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11439,4 +11491,30 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF420A7-D202-F346-88B0-96E88FA44224}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="112.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="232" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>